<commit_message>
fix: remove header in xlsx
</commit_message>
<xml_diff>
--- a/apps/server/excel-template/rundown.template.xlsx
+++ b/apps/server/excel-template/rundown.template.xlsx
@@ -5,70 +5,27 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CODE\Prods\ontime\apps\server\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CODE\Prods\ontime\apps\server\excel-template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4944B37-A038-4CE4-9A65-65E6A502A419}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C1B1869-9B5B-4CDA-9A0A-8CC1BD72EBAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Event schedule advanced" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
+  <extLst>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
-  <si>
-    <t>ⓘ Notes on import</t>
-  </si>
-  <si>
-    <t>ⓘ How to use</t>
-  </si>
-  <si>
-    <t>Ontime will import this spreasheet as a rundown in your project</t>
-  </si>
-  <si>
-    <t>1. Make your own copy of the spreadsheet by either File -&gt; Make a copy or File -&gt; Download -&gt; Microsoft Excel</t>
-  </si>
-  <si>
-    <t>- Each spreadsheet can only contain one rundown</t>
-  </si>
-  <si>
-    <t>2. Delete the table header with the Notes on import and How to use instructions</t>
-  </si>
-  <si>
-    <t>- You can have as many columns as necessary, Ontime only imports the columns you request</t>
-  </si>
-  <si>
-    <t>3. Remove any columns that are not necessary to your workflow</t>
-  </si>
-  <si>
-    <t>- The names of the worksheet and columns are given in Ontime on import</t>
-  </si>
-  <si>
-    <t>See documentation for spreadsheet import</t>
-  </si>
-  <si>
-    <t>https://docs.getontime.no/features/import-spreadsheet/</t>
-  </si>
-  <si>
-    <t>- Ontime creates an entry for every row on the table with a known Timer Type (see note on column header)</t>
-  </si>
-  <si>
-    <t>See documentation for Google Sheet import</t>
-  </si>
-  <si>
-    <t>https://docs.getontime.no/features/import-spreadsheet-gsheet/</t>
-  </si>
-  <si>
-    <t>- All fields in a row are optional, Ontime will fill in with default data as needed</t>
-  </si>
-  <si>
-    <t>ⓘ Hover over note tags to see additional help on column data</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Note</t>
   </si>
@@ -122,7 +79,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -138,41 +95,6 @@
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="17"/>
-      <color rgb="FF5B95F9"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color rgb="FF5B95F9"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="10"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FF3C78D8"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -219,18 +141,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="21" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
@@ -520,7 +435,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table_2" displayName="Table_2" ref="B12:Q13" insertRow="1" headerRowDxfId="18" dataDxfId="17" totalsRowDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table_2" displayName="Table_2" ref="B2:Q3" insertRow="1" headerRowDxfId="18" dataDxfId="17" totalsRowDxfId="16">
   <tableColumns count="16">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="ID" dataDxfId="15"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Cue" dataDxfId="14"/>
@@ -745,14 +660,14 @@
     <tabColor rgb="FF5B95F9"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:V13"/>
+  <dimension ref="A1:V3"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="12" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4.28515625" style="2" customWidth="1"/>
     <col min="2" max="2" width="7.7109375" style="2" customWidth="1"/>
@@ -796,308 +711,98 @@
       <c r="U1" s="1"/>
       <c r="V1" s="1"/>
     </row>
-    <row r="2" spans="1:22" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:22" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="M2" s="1"/>
+      <c r="L2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
       <c r="U2" s="1"/>
       <c r="V2" s="1"/>
     </row>
-    <row r="3" spans="1:22" ht="12.75" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:22" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
-      <c r="B3" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="7"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="6"/>
-      <c r="H3" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="M3" s="1"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="4"/>
+      <c r="Q3" s="4"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
       <c r="U3" s="1"/>
       <c r="V3" s="1"/>
     </row>
-    <row r="4" spans="1:22" ht="12.75" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="1"/>
-      <c r="B4" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="6"/>
-      <c r="H4" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="M4" s="1"/>
-      <c r="R4" s="1"/>
-      <c r="S4" s="1"/>
-      <c r="T4" s="1"/>
-      <c r="U4" s="1"/>
-      <c r="V4" s="1"/>
-    </row>
-    <row r="5" spans="1:22" ht="12.75" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="1"/>
-      <c r="B5" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="1"/>
-      <c r="F5" s="6"/>
-      <c r="H5" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="R5" s="1"/>
-      <c r="S5" s="1"/>
-      <c r="T5" s="1"/>
-      <c r="U5" s="1"/>
-      <c r="V5" s="1"/>
-    </row>
-    <row r="6" spans="1:22" ht="12.75" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="1"/>
-      <c r="B6" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="1"/>
-      <c r="F6" s="6"/>
-      <c r="H6" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="I6" s="1"/>
-      <c r="J6" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="R6" s="1"/>
-      <c r="S6" s="1"/>
-      <c r="T6" s="1"/>
-      <c r="U6" s="1"/>
-      <c r="V6" s="1"/>
-    </row>
-    <row r="7" spans="1:22" ht="12.75" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="1"/>
-      <c r="B7" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="1"/>
-      <c r="F7" s="6"/>
-      <c r="H7" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="I7" s="1"/>
-      <c r="J7" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="R7" s="1"/>
-      <c r="S7" s="1"/>
-      <c r="T7" s="1"/>
-      <c r="U7" s="1"/>
-      <c r="V7" s="1"/>
-    </row>
-    <row r="8" spans="1:22" ht="12.75" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="1"/>
-      <c r="B8" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="1"/>
-      <c r="F8" s="6"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
-      <c r="R8" s="1"/>
-      <c r="S8" s="1"/>
-      <c r="T8" s="1"/>
-      <c r="U8" s="1"/>
-      <c r="V8" s="1"/>
-    </row>
-    <row r="9" spans="1:22" ht="12.75" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
-      <c r="N9" s="1"/>
-      <c r="O9" s="1"/>
-      <c r="P9" s="1"/>
-      <c r="Q9" s="1"/>
-      <c r="R9" s="1"/>
-      <c r="S9" s="1"/>
-      <c r="T9" s="1"/>
-      <c r="U9" s="1"/>
-      <c r="V9" s="1"/>
-    </row>
-    <row r="10" spans="1:22" ht="12.75" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="1"/>
-      <c r="B10" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
-      <c r="O10" s="1"/>
-      <c r="P10" s="1"/>
-      <c r="Q10" s="1"/>
-      <c r="R10" s="1"/>
-      <c r="S10" s="1"/>
-      <c r="T10" s="1"/>
-      <c r="U10" s="1"/>
-      <c r="V10" s="1"/>
-    </row>
-    <row r="11" spans="1:22" ht="12.75" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
-      <c r="N11" s="1"/>
-      <c r="O11" s="1"/>
-      <c r="P11" s="1"/>
-      <c r="Q11" s="1"/>
-      <c r="R11" s="1"/>
-      <c r="S11" s="1"/>
-      <c r="T11" s="1"/>
-      <c r="U11" s="1"/>
-      <c r="V11" s="1"/>
-    </row>
-    <row r="12" spans="1:22" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A12" s="1"/>
-      <c r="B12" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="G12" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="H12" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="I12" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="J12" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="K12" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="L12" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="M12" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="N12" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="O12" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="P12" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q12" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="R12" s="1"/>
-      <c r="S12" s="1"/>
-      <c r="T12" s="1"/>
-      <c r="U12" s="1"/>
-      <c r="V12" s="1"/>
-    </row>
-    <row r="13" spans="1:22" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A13" s="1"/>
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="11"/>
-      <c r="K13" s="11"/>
-      <c r="L13" s="11"/>
-      <c r="M13" s="11"/>
-      <c r="N13" s="12"/>
-      <c r="O13" s="12"/>
-      <c r="P13" s="11"/>
-      <c r="Q13" s="11"/>
-      <c r="R13" s="1"/>
-      <c r="S13" s="1"/>
-      <c r="T13" s="1"/>
-      <c r="U13" s="1"/>
-      <c r="V13" s="1"/>
-    </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="M13" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="M3" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"none,load-next,play-next"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="L13" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="L3" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"count-down,count-up,clock,group-start,group-end,skip-import,milestone"</formula1>
     </dataValidation>
   </dataValidations>
-  <hyperlinks>
-    <hyperlink ref="J6" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="J7" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>